<commit_message>
Clustering for multidimensional Points
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="77">
   <si>
     <t>ID</t>
   </si>
@@ -29,46 +29,94 @@
     <t>3.5</t>
   </si>
   <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
     <t>4.9</t>
   </si>
   <si>
     <t>3.1</t>
   </si>
   <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
     <t>5.7</t>
   </si>
   <si>
     <t>2.8</t>
   </si>
   <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
     <t>6.3</t>
   </si>
   <si>
     <t>3.3</t>
   </si>
   <si>
+    <t>6.0</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
     <t>5.8</t>
   </si>
   <si>
     <t>2.7</t>
   </si>
   <si>
+    <t>1.9</t>
+  </si>
+  <si>
     <t>7.1</t>
   </si>
   <si>
     <t>3.0</t>
   </si>
   <si>
+    <t>5.9</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
     <t>2.9</t>
   </si>
   <si>
+    <t>5.6</t>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
+  <si>
     <t>6.5</t>
   </si>
   <si>
+    <t>2.2</t>
+  </si>
+  <si>
     <t>7.6</t>
   </si>
   <si>
-    <t>2.5</t>
+    <t>6.6</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>1.7</t>
   </si>
   <si>
     <t>7.3</t>
@@ -89,15 +137,36 @@
     <t>3.6</t>
   </si>
   <si>
+    <t>6.1</t>
+  </si>
+  <si>
     <t>3.2</t>
   </si>
   <si>
+    <t>2.0</t>
+  </si>
+  <si>
     <t>6.4</t>
   </si>
   <si>
+    <t>5.3</t>
+  </si>
+  <si>
     <t>6.8</t>
   </si>
   <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
     <t>7.7</t>
   </si>
   <si>
@@ -107,30 +176,21 @@
     <t>2.6</t>
   </si>
   <si>
+    <t>6.9</t>
+  </si>
+  <si>
     <t>4.8</t>
   </si>
   <si>
     <t>3.4</t>
   </si>
   <si>
-    <t>6.0</t>
-  </si>
-  <si>
-    <t>2.2</t>
-  </si>
-  <si>
-    <t>6.9</t>
-  </si>
-  <si>
-    <t>5.6</t>
+    <t>1.6</t>
   </si>
   <si>
     <t>6.2</t>
   </si>
   <si>
-    <t>6.1</t>
-  </si>
-  <si>
     <t>7.4</t>
   </si>
   <si>
@@ -140,58 +200,49 @@
     <t>4.3</t>
   </si>
   <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
     <t>4.0</t>
   </si>
   <si>
-    <t>5.9</t>
+    <t>1.2</t>
   </si>
   <si>
     <t>4.4</t>
   </si>
   <si>
+    <t>0.4</t>
+  </si>
+  <si>
     <t>3.9</t>
   </si>
   <si>
+    <t>0.3</t>
+  </si>
+  <si>
     <t>4.6</t>
   </si>
   <si>
-    <t>5.0</t>
-  </si>
-  <si>
-    <t>5.2</t>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>0.5</t>
   </si>
   <si>
     <t>4.7</t>
   </si>
   <si>
-    <t>4.1</t>
-  </si>
-  <si>
-    <t>5.5</t>
-  </si>
-  <si>
     <t>4.2</t>
   </si>
   <si>
-    <t>4.5</t>
-  </si>
-  <si>
-    <t>2.3</t>
-  </si>
-  <si>
-    <t>5.3</t>
+    <t>0.6</t>
   </si>
   <si>
     <t>7.0</t>
-  </si>
-  <si>
-    <t>2.4</t>
-  </si>
-  <si>
-    <t>6.6</t>
-  </si>
-  <si>
-    <t>2.0</t>
   </si>
 </sst>
 </file>
@@ -236,7 +287,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D151"/>
+  <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -263,16 +314,28 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>9.0</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -280,10 +343,16 @@
         <v>99.0</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5">
@@ -291,10 +360,16 @@
         <v>100.0</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6">
@@ -302,10 +377,16 @@
         <v>101.0</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7">
@@ -313,10 +394,16 @@
         <v>102.0</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -324,10 +411,16 @@
         <v>103.0</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9">
@@ -335,10 +428,16 @@
         <v>104.0</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10">
@@ -346,10 +445,16 @@
         <v>105.0</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11">
@@ -357,10 +462,16 @@
         <v>106.0</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12">
@@ -368,10 +479,16 @@
         <v>107.0</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
         <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13">
@@ -379,10 +496,16 @@
         <v>108.0</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14">
@@ -390,10 +513,16 @@
         <v>10.0</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="15">
@@ -401,10 +530,16 @@
         <v>109.0</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16">
@@ -412,10 +547,16 @@
         <v>110.0</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="17">
@@ -423,10 +564,16 @@
         <v>111.0</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="D17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="18">
@@ -434,10 +581,16 @@
         <v>112.0</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="19">
@@ -445,10 +598,16 @@
         <v>113.0</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="20">
@@ -456,10 +615,16 @@
         <v>114.0</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="21">
@@ -467,10 +632,16 @@
         <v>115.0</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>42</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="22">
@@ -478,10 +649,16 @@
         <v>116.0</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="23">
@@ -489,10 +666,16 @@
         <v>117.0</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>52</v>
+      </c>
+      <c r="D23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="24">
@@ -500,10 +683,16 @@
         <v>118.0</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>53</v>
+      </c>
+      <c r="D24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="25">
@@ -511,10 +700,16 @@
         <v>11.0</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>56</v>
+      </c>
+      <c r="D25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="26">
@@ -522,10 +717,16 @@
         <v>119.0</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="27">
@@ -533,10 +734,16 @@
         <v>120.0</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>25</v>
+        <v>42</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="28">
@@ -544,10 +751,16 @@
         <v>121.0</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="29">
@@ -555,10 +768,16 @@
         <v>122.0</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="D29" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="30">
@@ -566,10 +785,16 @@
         <v>123.0</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="31">
@@ -577,10 +802,16 @@
         <v>124.0</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="32">
@@ -588,10 +819,16 @@
         <v>125.0</v>
       </c>
       <c r="B32" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>42</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="33">
@@ -599,10 +836,16 @@
         <v>126.0</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="D33" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="34">
@@ -610,10 +853,16 @@
         <v>127.0</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="35">
@@ -621,10 +870,16 @@
         <v>128.0</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="D35" t="s">
+        <v>27</v>
+      </c>
+      <c r="E35" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="36">
@@ -632,10 +887,16 @@
         <v>12.0</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="37">
@@ -643,10 +904,16 @@
         <v>129.0</v>
       </c>
       <c r="B37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" t="s">
         <v>23</v>
       </c>
-      <c r="C37" t="s">
-        <v>14</v>
+      <c r="D37" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="38">
@@ -654,10 +921,16 @@
         <v>130.0</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="D38" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="39">
@@ -665,10 +938,16 @@
         <v>131.0</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C39" t="s">
-        <v>29</v>
+        <v>52</v>
+      </c>
+      <c r="D39" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="40">
@@ -676,10 +955,16 @@
         <v>132.0</v>
       </c>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C40" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="D40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="41">
@@ -687,10 +972,16 @@
         <v>133.0</v>
       </c>
       <c r="B41" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
         <v>9</v>
-      </c>
-      <c r="C41" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="42">
@@ -698,10 +989,16 @@
         <v>134.0</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>30</v>
+        <v>53</v>
+      </c>
+      <c r="D42" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="43">
@@ -709,10 +1006,16 @@
         <v>135.0</v>
       </c>
       <c r="B43" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C43" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D43" t="s">
+        <v>41</v>
+      </c>
+      <c r="E43" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="44">
@@ -720,10 +1023,16 @@
         <v>136.0</v>
       </c>
       <c r="B44" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C44" t="s">
-        <v>32</v>
+        <v>56</v>
+      </c>
+      <c r="D44" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="45">
@@ -731,10 +1040,16 @@
         <v>137.0</v>
       </c>
       <c r="B45" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D45" t="s">
+        <v>47</v>
+      </c>
+      <c r="E45" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="46">
@@ -742,10 +1057,16 @@
         <v>138.0</v>
       </c>
       <c r="B46" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C46" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D46" t="s">
+        <v>55</v>
+      </c>
+      <c r="E46" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="47">
@@ -753,10 +1074,16 @@
         <v>13.0</v>
       </c>
       <c r="B47" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C47" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D47" t="s">
+        <v>62</v>
+      </c>
+      <c r="E47" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="48">
@@ -764,10 +1091,16 @@
         <v>139.0</v>
       </c>
       <c r="B48" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="C48" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D48" t="s">
+        <v>37</v>
+      </c>
+      <c r="E48" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="49">
@@ -775,10 +1108,16 @@
         <v>140.0</v>
       </c>
       <c r="B49" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C49" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D49" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="50">
@@ -786,10 +1125,16 @@
         <v>141.0</v>
       </c>
       <c r="B50" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="C50" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D50" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="51">
@@ -797,10 +1142,16 @@
         <v>142.0</v>
       </c>
       <c r="B51" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C51" t="s">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="D51" t="s">
+        <v>3</v>
+      </c>
+      <c r="E51" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="52">
@@ -808,10 +1159,16 @@
         <v>143.0</v>
       </c>
       <c r="B52" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="C52" t="s">
-        <v>25</v>
+        <v>42</v>
+      </c>
+      <c r="D52" t="s">
+        <v>24</v>
+      </c>
+      <c r="E52" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="53">
@@ -819,10 +1176,16 @@
         <v>144.0</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C53" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="D53" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="54">
@@ -830,10 +1193,16 @@
         <v>145.0</v>
       </c>
       <c r="B54" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C54" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D54" t="s">
+        <v>63</v>
+      </c>
+      <c r="E54" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="55">
@@ -841,10 +1210,16 @@
         <v>146.0</v>
       </c>
       <c r="B55" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C55" t="s">
         <v>18</v>
+      </c>
+      <c r="D55" t="s">
+        <v>48</v>
+      </c>
+      <c r="E55" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="56">
@@ -852,10 +1227,16 @@
         <v>147.0</v>
       </c>
       <c r="B56" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C56" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E56" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="57">
@@ -863,10 +1244,16 @@
         <v>148.0</v>
       </c>
       <c r="B57" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57" t="s">
+        <v>56</v>
+      </c>
+      <c r="D57" t="s">
         <v>37</v>
       </c>
-      <c r="C57" t="s">
-        <v>32</v>
+      <c r="E57" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="58">
@@ -874,10 +1261,16 @@
         <v>14.0</v>
       </c>
       <c r="B58" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C58" t="s">
-        <v>42</v>
+        <v>64</v>
+      </c>
+      <c r="D58" t="s">
+        <v>65</v>
+      </c>
+      <c r="E58" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="59">
@@ -885,10 +1278,16 @@
         <v>149.0</v>
       </c>
       <c r="B59" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="C59" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E59" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="60">
@@ -896,10 +1295,16 @@
         <v>15.0</v>
       </c>
       <c r="B60" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C60" t="s">
-        <v>44</v>
+        <v>66</v>
+      </c>
+      <c r="D60" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="61">
@@ -907,10 +1312,16 @@
         <v>16.0</v>
       </c>
       <c r="B61" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C61" t="s">
-        <v>45</v>
+        <v>68</v>
+      </c>
+      <c r="D61" t="s">
+        <v>14</v>
+      </c>
+      <c r="E61" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="62">
@@ -923,16 +1334,28 @@
       <c r="C62" t="s">
         <v>4</v>
       </c>
+      <c r="D62" t="s">
+        <v>5</v>
+      </c>
+      <c r="E62" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
         <v>18.0</v>
       </c>
       <c r="B63" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C63" t="s">
-        <v>29</v>
+        <v>52</v>
+      </c>
+      <c r="D63" t="s">
+        <v>34</v>
+      </c>
+      <c r="E63" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="64">
@@ -940,10 +1363,16 @@
         <v>1.0</v>
       </c>
       <c r="B64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" t="s">
+        <v>23</v>
+      </c>
+      <c r="D64" t="s">
         <v>5</v>
       </c>
-      <c r="C64" t="s">
-        <v>14</v>
+      <c r="E64" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="65">
@@ -954,7 +1383,13 @@
         <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>29</v>
+        <v>52</v>
+      </c>
+      <c r="D65" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="66">
@@ -962,10 +1397,16 @@
         <v>20.0</v>
       </c>
       <c r="B66" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C66" t="s">
-        <v>32</v>
+        <v>56</v>
+      </c>
+      <c r="D66" t="s">
+        <v>34</v>
+      </c>
+      <c r="E66" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="67">
@@ -976,7 +1417,13 @@
         <v>3</v>
       </c>
       <c r="C67" t="s">
-        <v>22</v>
+        <v>38</v>
+      </c>
+      <c r="D67" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="68">
@@ -984,10 +1431,16 @@
         <v>22.0</v>
       </c>
       <c r="B68" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="C68" t="s">
-        <v>24</v>
+        <v>40</v>
+      </c>
+      <c r="D68" t="s">
+        <v>71</v>
+      </c>
+      <c r="E68" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="69">
@@ -998,7 +1451,13 @@
         <v>3</v>
       </c>
       <c r="C69" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="D69" t="s">
+        <v>34</v>
+      </c>
+      <c r="E69" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="70">
@@ -1006,10 +1465,16 @@
         <v>24.0</v>
       </c>
       <c r="B70" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="C70" t="s">
-        <v>32</v>
+        <v>56</v>
+      </c>
+      <c r="D70" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="71">
@@ -1017,10 +1482,16 @@
         <v>25.0</v>
       </c>
       <c r="B71" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C71" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D71" t="s">
+        <v>57</v>
+      </c>
+      <c r="E71" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="72">
@@ -1028,10 +1499,16 @@
         <v>26.0</v>
       </c>
       <c r="B72" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C72" t="s">
-        <v>32</v>
+        <v>56</v>
+      </c>
+      <c r="D72" t="s">
+        <v>57</v>
+      </c>
+      <c r="E72" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="73">
@@ -1039,10 +1516,16 @@
         <v>27.0</v>
       </c>
       <c r="B73" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="C73" t="s">
         <v>4</v>
+      </c>
+      <c r="D73" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="74">
@@ -1050,10 +1533,16 @@
         <v>28.0</v>
       </c>
       <c r="B74" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="C74" t="s">
-        <v>32</v>
+        <v>56</v>
+      </c>
+      <c r="D74" t="s">
+        <v>5</v>
+      </c>
+      <c r="E74" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="75">
@@ -1061,10 +1550,16 @@
         <v>2.0</v>
       </c>
       <c r="B75" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="C75" t="s">
-        <v>25</v>
+        <v>42</v>
+      </c>
+      <c r="D75" t="s">
+        <v>14</v>
+      </c>
+      <c r="E75" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="76">
@@ -1072,10 +1567,16 @@
         <v>29.0</v>
       </c>
       <c r="B76" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="C76" t="s">
-        <v>25</v>
+        <v>42</v>
+      </c>
+      <c r="D76" t="s">
+        <v>57</v>
+      </c>
+      <c r="E76" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="77">
@@ -1083,9 +1584,15 @@
         <v>30.0</v>
       </c>
       <c r="B77" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="C77" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" t="s">
+        <v>57</v>
+      </c>
+      <c r="E77" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1094,10 +1601,16 @@
         <v>31.0</v>
       </c>
       <c r="B78" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C78" t="s">
-        <v>32</v>
+        <v>56</v>
+      </c>
+      <c r="D78" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="79">
@@ -1105,10 +1618,16 @@
         <v>32.0</v>
       </c>
       <c r="B79" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="C79" t="s">
-        <v>50</v>
+        <v>13</v>
+      </c>
+      <c r="D79" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="80">
@@ -1116,10 +1635,16 @@
         <v>33.0</v>
       </c>
       <c r="B80" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C80" t="s">
-        <v>52</v>
+        <v>74</v>
+      </c>
+      <c r="D80" t="s">
+        <v>5</v>
+      </c>
+      <c r="E80" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="81">
@@ -1127,10 +1652,16 @@
         <v>34.0</v>
       </c>
       <c r="B81" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C81" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D81" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="82">
@@ -1138,10 +1669,16 @@
         <v>35.0</v>
       </c>
       <c r="B82" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C82" t="s">
-        <v>25</v>
+        <v>42</v>
+      </c>
+      <c r="D82" t="s">
+        <v>65</v>
+      </c>
+      <c r="E82" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="83">
@@ -1149,10 +1686,16 @@
         <v>36.0</v>
       </c>
       <c r="B83" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C83" t="s">
         <v>4</v>
+      </c>
+      <c r="D83" t="s">
+        <v>14</v>
+      </c>
+      <c r="E83" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="84">
@@ -1160,10 +1703,16 @@
         <v>37.0</v>
       </c>
       <c r="B84" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C84" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D84" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="85">
@@ -1171,10 +1720,16 @@
         <v>38.0</v>
       </c>
       <c r="B85" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="C85" t="s">
+        <v>23</v>
+      </c>
+      <c r="D85" t="s">
         <v>14</v>
+      </c>
+      <c r="E85" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="86">
@@ -1182,9 +1737,15 @@
         <v>3.0</v>
       </c>
       <c r="B86" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="C86" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1196,7 +1757,13 @@
         <v>3</v>
       </c>
       <c r="C87" t="s">
-        <v>32</v>
+        <v>56</v>
+      </c>
+      <c r="D87" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="88">
@@ -1204,10 +1771,16 @@
         <v>40.0</v>
       </c>
       <c r="B88" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C88" t="s">
         <v>4</v>
+      </c>
+      <c r="D88" t="s">
+        <v>14</v>
+      </c>
+      <c r="E88" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="89">
@@ -1215,10 +1788,16 @@
         <v>41.0</v>
       </c>
       <c r="B89" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="C89" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="D89" t="s">
+        <v>14</v>
+      </c>
+      <c r="E89" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="90">
@@ -1226,10 +1805,16 @@
         <v>42.0</v>
       </c>
       <c r="B90" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="C90" t="s">
-        <v>25</v>
+        <v>42</v>
+      </c>
+      <c r="D90" t="s">
+        <v>14</v>
+      </c>
+      <c r="E90" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="91">
@@ -1237,10 +1822,16 @@
         <v>43.0</v>
       </c>
       <c r="B91" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C91" t="s">
         <v>4</v>
+      </c>
+      <c r="D91" t="s">
+        <v>57</v>
+      </c>
+      <c r="E91" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="92">
@@ -1251,7 +1842,13 @@
         <v>3</v>
       </c>
       <c r="C92" t="s">
-        <v>29</v>
+        <v>52</v>
+      </c>
+      <c r="D92" t="s">
+        <v>21</v>
+      </c>
+      <c r="E92" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="93">
@@ -1259,10 +1856,16 @@
         <v>45.0</v>
       </c>
       <c r="B93" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="C93" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D93" t="s">
+        <v>5</v>
+      </c>
+      <c r="E93" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="94">
@@ -1273,7 +1876,13 @@
         <v>3</v>
       </c>
       <c r="C94" t="s">
-        <v>29</v>
+        <v>52</v>
+      </c>
+      <c r="D94" t="s">
+        <v>57</v>
+      </c>
+      <c r="E94" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="95">
@@ -1281,10 +1890,16 @@
         <v>47.0</v>
       </c>
       <c r="B95" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="C95" t="s">
-        <v>25</v>
+        <v>42</v>
+      </c>
+      <c r="D95" t="s">
+        <v>5</v>
+      </c>
+      <c r="E95" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="96">
@@ -1292,10 +1907,16 @@
         <v>48.0</v>
       </c>
       <c r="B96" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C96" t="s">
-        <v>22</v>
+        <v>38</v>
+      </c>
+      <c r="D96" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="97">
@@ -1303,10 +1924,16 @@
         <v>4.0</v>
       </c>
       <c r="B97" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C97" t="s">
-        <v>24</v>
+        <v>40</v>
+      </c>
+      <c r="D97" t="s">
+        <v>5</v>
+      </c>
+      <c r="E97" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="98">
@@ -1314,10 +1941,16 @@
         <v>49.0</v>
       </c>
       <c r="B98" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C98" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="D98" t="s">
+        <v>5</v>
+      </c>
+      <c r="E98" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="99">
@@ -1325,10 +1958,16 @@
         <v>50.0</v>
       </c>
       <c r="B99" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="C99" t="s">
-        <v>25</v>
+        <v>42</v>
+      </c>
+      <c r="D99" t="s">
+        <v>73</v>
+      </c>
+      <c r="E99" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="100">
@@ -1336,10 +1975,16 @@
         <v>51.0</v>
       </c>
       <c r="B100" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C100" t="s">
-        <v>25</v>
+        <v>42</v>
+      </c>
+      <c r="D100" t="s">
+        <v>33</v>
+      </c>
+      <c r="E100" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="101">
@@ -1347,10 +1992,16 @@
         <v>52.0</v>
       </c>
       <c r="B101" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="C101" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D101" t="s">
+        <v>7</v>
+      </c>
+      <c r="E101" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="102">
@@ -1358,10 +2009,16 @@
         <v>53.0</v>
       </c>
       <c r="B102" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C102" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="D102" t="s">
+        <v>64</v>
+      </c>
+      <c r="E102" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="103">
@@ -1369,10 +2026,16 @@
         <v>54.0</v>
       </c>
       <c r="B103" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C103" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="D103" t="s">
+        <v>70</v>
+      </c>
+      <c r="E103" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="104">
@@ -1380,10 +2043,16 @@
         <v>55.0</v>
       </c>
       <c r="B104" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C104" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="D104" t="s">
+        <v>33</v>
+      </c>
+      <c r="E104" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="105">
@@ -1391,10 +2060,16 @@
         <v>56.0</v>
       </c>
       <c r="B105" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C105" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="D105" t="s">
+        <v>73</v>
+      </c>
+      <c r="E105" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="106">
@@ -1402,10 +2077,16 @@
         <v>57.0</v>
       </c>
       <c r="B106" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C106" t="s">
-        <v>57</v>
+        <v>49</v>
+      </c>
+      <c r="D106" t="s">
+        <v>16</v>
+      </c>
+      <c r="E106" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="107">
@@ -1413,10 +2094,16 @@
         <v>58.0</v>
       </c>
       <c r="B107" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C107" t="s">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="D107" t="s">
+        <v>70</v>
+      </c>
+      <c r="E107" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="108">
@@ -1424,10 +2111,16 @@
         <v>5.0</v>
       </c>
       <c r="B108" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C108" t="s">
-        <v>45</v>
+        <v>68</v>
+      </c>
+      <c r="D108" t="s">
+        <v>34</v>
+      </c>
+      <c r="E108" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="109">
@@ -1435,10 +2128,16 @@
         <v>59.0</v>
       </c>
       <c r="B109" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="C109" t="s">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="D109" t="s">
+        <v>68</v>
+      </c>
+      <c r="E109" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="110">
@@ -1446,10 +2145,16 @@
         <v>60.0</v>
       </c>
       <c r="B110" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C110" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="D110" t="s">
+        <v>4</v>
+      </c>
+      <c r="E110" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="111">
@@ -1457,10 +2162,16 @@
         <v>61.0</v>
       </c>
       <c r="B111" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="C111" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D111" t="s">
+        <v>74</v>
+      </c>
+      <c r="E111" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="112">
@@ -1468,10 +2179,16 @@
         <v>62.0</v>
       </c>
       <c r="B112" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C112" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="D112" t="s">
+        <v>64</v>
+      </c>
+      <c r="E112" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="113">
@@ -1479,10 +2196,16 @@
         <v>63.0</v>
       </c>
       <c r="B113" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C113" t="s">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="D113" t="s">
+        <v>73</v>
+      </c>
+      <c r="E113" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="114">
@@ -1490,10 +2213,16 @@
         <v>64.0</v>
       </c>
       <c r="B114" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C114" t="s">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="D114" t="s">
+        <v>40</v>
+      </c>
+      <c r="E114" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="115">
@@ -1501,10 +2230,16 @@
         <v>65.0</v>
       </c>
       <c r="B115" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C115" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D115" t="s">
+        <v>66</v>
+      </c>
+      <c r="E115" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="116">
@@ -1512,10 +2247,16 @@
         <v>66.0</v>
       </c>
       <c r="B116" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C116" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D116" t="s">
+        <v>33</v>
+      </c>
+      <c r="E116" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="117">
@@ -1523,10 +2264,16 @@
         <v>67.0</v>
       </c>
       <c r="B117" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C117" t="s">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="D117" t="s">
+        <v>13</v>
+      </c>
+      <c r="E117" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="118">
@@ -1534,10 +2281,16 @@
         <v>68.0</v>
       </c>
       <c r="B118" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="C118" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="D118" t="s">
+        <v>33</v>
+      </c>
+      <c r="E118" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="119">
@@ -1545,10 +2298,16 @@
         <v>6.0</v>
       </c>
       <c r="B119" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="C119" t="s">
-        <v>32</v>
+        <v>56</v>
+      </c>
+      <c r="D119" t="s">
+        <v>5</v>
+      </c>
+      <c r="E119" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="120">
@@ -1556,10 +2315,16 @@
         <v>69.0</v>
       </c>
       <c r="B120" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C120" t="s">
         <v>18</v>
+      </c>
+      <c r="D120" t="s">
+        <v>68</v>
+      </c>
+      <c r="E120" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="121">
@@ -1567,10 +2332,16 @@
         <v>70.0</v>
       </c>
       <c r="B121" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="C121" t="s">
-        <v>25</v>
+        <v>42</v>
+      </c>
+      <c r="D121" t="s">
+        <v>55</v>
+      </c>
+      <c r="E121" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="122">
@@ -1578,10 +2349,16 @@
         <v>71.0</v>
       </c>
       <c r="B122" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C122" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="D122" t="s">
+        <v>64</v>
+      </c>
+      <c r="E122" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="123">
@@ -1589,10 +2366,16 @@
         <v>72.0</v>
       </c>
       <c r="B123" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C123" t="s">
         <v>18</v>
+      </c>
+      <c r="D123" t="s">
+        <v>7</v>
+      </c>
+      <c r="E123" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="124">
@@ -1600,10 +2383,16 @@
         <v>73.0</v>
       </c>
       <c r="B124" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C124" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="D124" t="s">
+        <v>73</v>
+      </c>
+      <c r="E124" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="125">
@@ -1611,10 +2400,16 @@
         <v>74.0</v>
       </c>
       <c r="B125" t="s">
+        <v>44</v>
+      </c>
+      <c r="C125" t="s">
         <v>26</v>
       </c>
-      <c r="C125" t="s">
-        <v>15</v>
+      <c r="D125" t="s">
+        <v>61</v>
+      </c>
+      <c r="E125" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="126">
@@ -1622,10 +2417,16 @@
         <v>75.0</v>
       </c>
       <c r="B126" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C126" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D126" t="s">
+        <v>66</v>
+      </c>
+      <c r="E126" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="127">
@@ -1633,10 +2434,16 @@
         <v>76.0</v>
       </c>
       <c r="B127" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="C127" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="D127" t="s">
+        <v>55</v>
+      </c>
+      <c r="E127" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="128">
@@ -1644,10 +2451,16 @@
         <v>77.0</v>
       </c>
       <c r="B128" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C128" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D128" t="s">
+        <v>48</v>
+      </c>
+      <c r="E128" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="129">
@@ -1655,10 +2468,16 @@
         <v>78.0</v>
       </c>
       <c r="B129" t="s">
+        <v>17</v>
+      </c>
+      <c r="C129" t="s">
+        <v>26</v>
+      </c>
+      <c r="D129" t="s">
         <v>33</v>
       </c>
-      <c r="C129" t="s">
-        <v>15</v>
+      <c r="E129" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="130">
@@ -1666,10 +2485,16 @@
         <v>7.0</v>
       </c>
       <c r="B130" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C130" t="s">
-        <v>32</v>
+        <v>56</v>
+      </c>
+      <c r="D130" t="s">
+        <v>9</v>
+      </c>
+      <c r="E130" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="131">
@@ -1677,10 +2502,16 @@
         <v>79.0</v>
       </c>
       <c r="B131" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C131" t="s">
-        <v>30</v>
+        <v>53</v>
+      </c>
+      <c r="D131" t="s">
+        <v>4</v>
+      </c>
+      <c r="E131" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="132">
@@ -1688,10 +2519,16 @@
         <v>80.0</v>
       </c>
       <c r="B132" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C132" t="s">
-        <v>57</v>
+        <v>49</v>
+      </c>
+      <c r="D132" t="s">
+        <v>52</v>
+      </c>
+      <c r="E132" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="133">
@@ -1699,10 +2536,16 @@
         <v>81.0</v>
       </c>
       <c r="B133" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C133" t="s">
-        <v>57</v>
+        <v>49</v>
+      </c>
+      <c r="D133" t="s">
+        <v>38</v>
+      </c>
+      <c r="E133" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="134">
@@ -1710,10 +2553,16 @@
         <v>82.0</v>
       </c>
       <c r="B134" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C134" t="s">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="D134" t="s">
+        <v>68</v>
+      </c>
+      <c r="E134" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="135">
@@ -1721,10 +2570,16 @@
         <v>83.0</v>
       </c>
       <c r="B135" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C135" t="s">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="D135" t="s">
+        <v>3</v>
+      </c>
+      <c r="E135" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="136">
@@ -1732,10 +2587,16 @@
         <v>84.0</v>
       </c>
       <c r="B136" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C136" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D136" t="s">
+        <v>33</v>
+      </c>
+      <c r="E136" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="137">
@@ -1743,10 +2604,16 @@
         <v>85.0</v>
       </c>
       <c r="B137" t="s">
+        <v>17</v>
+      </c>
+      <c r="C137" t="s">
+        <v>56</v>
+      </c>
+      <c r="D137" t="s">
         <v>33</v>
       </c>
-      <c r="C137" t="s">
-        <v>32</v>
+      <c r="E137" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="138">
@@ -1754,10 +2621,16 @@
         <v>86.0</v>
       </c>
       <c r="B138" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C138" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D138" t="s">
+        <v>73</v>
+      </c>
+      <c r="E138" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="139">
@@ -1765,10 +2638,16 @@
         <v>87.0</v>
       </c>
       <c r="B139" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C139" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="D139" t="s">
+        <v>66</v>
+      </c>
+      <c r="E139" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="140">
@@ -1776,9 +2655,15 @@
         <v>88.0</v>
       </c>
       <c r="B140" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C140" t="s">
+        <v>23</v>
+      </c>
+      <c r="D140" t="s">
+        <v>13</v>
+      </c>
+      <c r="E140" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1787,10 +2672,16 @@
         <v>8.0</v>
       </c>
       <c r="B141" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="C141" t="s">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="D141" t="s">
+        <v>5</v>
+      </c>
+      <c r="E141" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="142">
@@ -1798,10 +2689,16 @@
         <v>89.0</v>
       </c>
       <c r="B142" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C142" t="s">
         <v>18</v>
+      </c>
+      <c r="D142" t="s">
+        <v>64</v>
+      </c>
+      <c r="E142" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="143">
@@ -1809,10 +2706,16 @@
         <v>90.0</v>
       </c>
       <c r="B143" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C143" t="s">
-        <v>30</v>
+        <v>53</v>
+      </c>
+      <c r="D143" t="s">
+        <v>66</v>
+      </c>
+      <c r="E143" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="144">
@@ -1820,10 +2723,16 @@
         <v>91.0</v>
       </c>
       <c r="B144" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C144" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D144" t="s">
+        <v>70</v>
+      </c>
+      <c r="E144" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="145">
@@ -1831,10 +2740,16 @@
         <v>92.0</v>
       </c>
       <c r="B145" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C145" t="s">
-        <v>30</v>
+        <v>53</v>
+      </c>
+      <c r="D145" t="s">
+        <v>64</v>
+      </c>
+      <c r="E145" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="146">
@@ -1842,10 +2757,16 @@
         <v>93.0</v>
       </c>
       <c r="B146" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C146" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="D146" t="s">
+        <v>16</v>
+      </c>
+      <c r="E146" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="147">
@@ -1853,10 +2774,16 @@
         <v>94.0</v>
       </c>
       <c r="B147" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C147" t="s">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="D147" t="s">
+        <v>74</v>
+      </c>
+      <c r="E147" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="148">
@@ -1864,10 +2791,16 @@
         <v>95.0</v>
       </c>
       <c r="B148" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C148" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D148" t="s">
+        <v>74</v>
+      </c>
+      <c r="E148" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="149">
@@ -1875,10 +2808,16 @@
         <v>96.0</v>
       </c>
       <c r="B149" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C149" t="s">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="D149" t="s">
+        <v>74</v>
+      </c>
+      <c r="E149" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="150">
@@ -1886,10 +2825,16 @@
         <v>97.0</v>
       </c>
       <c r="B150" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="C150" t="s">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="D150" t="s">
+        <v>61</v>
+      </c>
+      <c r="E150" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="151">
@@ -1901,6 +2846,12 @@
       </c>
       <c r="C151" t="s">
         <v>18</v>
+      </c>
+      <c r="D151" t="s">
+        <v>23</v>
+      </c>
+      <c r="E151" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>